<commit_message>
Last run before holiday
Changes data in and out
</commit_message>
<xml_diff>
--- a/thesis/main_new_formulation/sets.xlsx
+++ b/thesis/main_new_formulation/sets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cami/Documents/GitHub/pyesm_tesi/thesis/main_new_formulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60721998-D2C6-F847-9074-FB1061AB21D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58579A1-6157-F047-B1D0-3283C6C431D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_set_days" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="76">
   <si>
     <t>days_names</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Natural Gas</t>
-  </si>
-  <si>
-    <t>BEV battery charge</t>
   </si>
   <si>
     <t>BEV battery discharge</t>
@@ -773,10 +770,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -834,11 +831,6 @@
     <row r="11" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -850,11 +842,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -869,7 +864,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>17</v>
@@ -880,7 +875,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
@@ -891,7 +886,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -902,7 +897,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -913,7 +908,7 @@
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
@@ -924,7 +919,7 @@
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -935,7 +930,7 @@
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
@@ -946,7 +941,7 @@
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
@@ -957,7 +952,7 @@
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
@@ -968,7 +963,7 @@
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>17</v>
@@ -979,7 +974,7 @@
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>17</v>
@@ -990,7 +985,7 @@
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -1001,7 +996,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
@@ -1012,7 +1007,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -1023,7 +1018,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>17</v>
@@ -1034,7 +1029,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -1045,7 +1040,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
@@ -1056,7 +1051,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>17</v>
@@ -1099,7 +1094,7 @@
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>17</v>
@@ -1108,12 +1103,12 @@
         <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
@@ -1122,12 +1117,12 @@
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
@@ -1136,12 +1131,12 @@
         <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -1150,12 +1145,12 @@
         <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
@@ -1164,12 +1159,12 @@
         <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>17</v>
@@ -1178,12 +1173,12 @@
         <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
@@ -1192,12 +1187,12 @@
         <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
@@ -1206,12 +1201,12 @@
         <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
@@ -1220,12 +1215,12 @@
         <v>17</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>17</v>
@@ -1234,12 +1229,12 @@
         <v>17</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>17</v>
@@ -1248,12 +1243,12 @@
         <v>17</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -1262,12 +1257,12 @@
         <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
@@ -1276,12 +1271,12 @@
         <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -1290,12 +1285,12 @@
         <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>17</v>
@@ -1304,12 +1299,12 @@
         <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -1318,12 +1313,12 @@
         <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
@@ -1332,12 +1327,12 @@
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>17</v>
@@ -1346,12 +1341,12 @@
         <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>17</v>
@@ -1360,12 +1355,12 @@
         <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>17</v>
@@ -1374,12 +1369,12 @@
         <v>17</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>17</v>
@@ -1388,12 +1383,12 @@
         <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>17</v>
@@ -1402,12 +1397,12 @@
         <v>17</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>17</v>
@@ -1416,7 +1411,7 @@
         <v>17</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1441,7 +1436,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>